<commit_message>
Finalized process_tokens_and_dependencies_cleaned.py after a loong time.
</commit_message>
<xml_diff>
--- a/data/external/book_data_external.xlsx
+++ b/data/external/book_data_external.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7B2591-52E2-4C46-AA1C-FFAFC4BFAB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFAC828-B24D-4BE0-A182-BF8C7C04B3B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -706,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Minor changes to book_data_external.xlsx and how it is handled in scrape_goodreads_reviews.py and data_processing_helper_functions.py.
</commit_message>
<xml_diff>
--- a/data/external/book_data_external.xlsx
+++ b/data/external/book_data_external.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFAC828-B24D-4BE0-A182-BF8C7C04B3B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADFC94E-18F3-4AAF-BE1D-CAF0D53A42BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
   <si>
     <t>http</t>
   </si>
@@ -132,12 +132,6 @@
     <t>Snow</t>
   </si>
   <si>
-    <t>Erdağ M. Göknar</t>
-  </si>
-  <si>
-    <t>Maureen Freely</t>
-  </si>
-  <si>
     <t>The Museum of Innocence</t>
   </si>
   <si>
@@ -150,15 +144,6 @@
     <t>The White Castle</t>
   </si>
   <si>
-    <t>Victoria Rowe Holbrook</t>
-  </si>
-  <si>
-    <t>Ekin Oklap</t>
-  </si>
-  <si>
-    <t>not found</t>
-  </si>
-  <si>
     <t>A Strangeness in My Mind</t>
   </si>
   <si>
@@ -168,9 +153,6 @@
     <t>The New Life</t>
   </si>
   <si>
-    <t>Güneli Gün</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/157993</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t xml:space="preserve">Antoine de Saint-Exupéry, </t>
   </si>
   <si>
-    <t>Richard Howard</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/52036</t>
   </si>
   <si>
@@ -192,18 +171,12 @@
     <t>Hermann Hesse</t>
   </si>
   <si>
-    <t>Hilda Rosner</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/16631</t>
   </si>
   <si>
     <t>Steppenwolf</t>
   </si>
   <si>
-    <t>Basil Creighton</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/117833</t>
   </si>
   <si>
@@ -213,21 +186,12 @@
     <t>Mikhail Bulgakov</t>
   </si>
   <si>
-    <t>Katherine Tiernan O'Connor</t>
-  </si>
-  <si>
-    <t>translator_first</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/16640</t>
   </si>
   <si>
     <t>The Sorrows of Young Werther</t>
   </si>
   <si>
-    <t>R. Dillon Boylan</t>
-  </si>
-  <si>
     <t>Johann Wolfgang von Goethe</t>
   </si>
   <si>
@@ -240,18 +204,12 @@
     <t>https://www.goodreads.com/book/show/17690</t>
   </si>
   <si>
-    <t>Willa Muir</t>
-  </si>
-  <si>
     <t>The Stranger</t>
   </si>
   <si>
     <t>Albert Camus</t>
   </si>
   <si>
-    <t>Matthew Ward</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/49552</t>
   </si>
   <si>
@@ -273,12 +231,6 @@
     <t>Gabriel Garcia Marquez</t>
   </si>
   <si>
-    <t>Gregory Rabassa</t>
-  </si>
-  <si>
-    <t>David McDuff</t>
-  </si>
-  <si>
     <t>https://www.goodreads.com/book/show/527756</t>
   </si>
   <si>
@@ -286,9 +238,6 @@
   </si>
   <si>
     <t>Robert Musil</t>
-  </si>
-  <si>
-    <t>Sophie Wilkins</t>
   </si>
   <si>
     <t>h10</t>
@@ -706,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -738,9 +687,7 @@
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>63</v>
-      </c>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -758,9 +705,6 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -778,9 +722,6 @@
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -793,13 +734,10 @@
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,13 +751,10 @@
         <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -833,13 +768,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,13 +785,10 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -873,13 +802,10 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -893,13 +819,10 @@
         <v>18</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -913,213 +836,180 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran the whole pipeline after finishing gather_book_level_statistics.py
</commit_message>
<xml_diff>
--- a/data/external/book_data_external.xlsx
+++ b/data/external/book_data_external.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADFC94E-18F3-4AAF-BE1D-CAF0D53A42BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA5731-86CA-4658-B0BA-CF71E687345B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
     <col min="8" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -687,9 +687,8 @@
       <c r="E1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -706,7 +705,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -723,7 +722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -740,7 +739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>32</v>
       </c>
@@ -757,7 +756,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -774,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
@@ -791,7 +790,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -808,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -825,7 +824,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>29</v>
       </c>
@@ -842,7 +841,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>71</v>
       </c>
@@ -859,7 +858,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>72</v>
       </c>
@@ -876,7 +875,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>73</v>
       </c>
@@ -893,7 +892,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>74</v>
       </c>
@@ -910,7 +909,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>75</v>
       </c>
@@ -927,7 +926,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
Imported the final version of the analysis and the required data sources.
</commit_message>
<xml_diff>
--- a/data/external/book_data_external.xlsx
+++ b/data/external/book_data_external.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\bachelors_paper_proof_of_concept\data\external\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgen\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECEA5731-86CA-4658-B0BA-CF71E687345B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80197CBA-22BD-4B63-BC48-A43DADC9BE4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="60" windowWidth="19180" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="582">
   <si>
     <t>http</t>
   </si>
@@ -298,6 +298,1479 @@
   </si>
   <si>
     <t>b19</t>
+  </si>
+  <si>
+    <t>The Count of Monte Cristo</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/7126</t>
+  </si>
+  <si>
+    <t>Don Quixote</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/3836</t>
+  </si>
+  <si>
+    <t>Candide</t>
+  </si>
+  <si>
+    <t>The Metamorphosis</t>
+  </si>
+  <si>
+    <t>The Brothers Karamazov</t>
+  </si>
+  <si>
+    <t>The Woman in the Dunes</t>
+  </si>
+  <si>
+    <t>The Unbearable Lightness of Being</t>
+  </si>
+  <si>
+    <t>Madame Bovary</t>
+  </si>
+  <si>
+    <t>Love in the Times of Cholera</t>
+  </si>
+  <si>
+    <t>War and Peace</t>
+  </si>
+  <si>
+    <t>Anna Karenina</t>
+  </si>
+  <si>
+    <t>The Name of the Rose</t>
+  </si>
+  <si>
+    <t>Quo Vadis</t>
+  </si>
+  <si>
+    <t>The Book of Disquiet</t>
+  </si>
+  <si>
+    <t>The Wind-Up Bird Chronicle</t>
+  </si>
+  <si>
+    <t>All Quiet on the Western Front</t>
+  </si>
+  <si>
+    <t>The Alchemist</t>
+  </si>
+  <si>
+    <t>The Magic Mountain</t>
+  </si>
+  <si>
+    <t>The Girl with the Dragon Tattoo</t>
+  </si>
+  <si>
+    <t>The Plague</t>
+  </si>
+  <si>
+    <t>Dead Souls</t>
+  </si>
+  <si>
+    <t>Blindness</t>
+  </si>
+  <si>
+    <t>Norwegian Wood</t>
+  </si>
+  <si>
+    <t>Kafka on the Shore</t>
+  </si>
+  <si>
+    <t>Hunger</t>
+  </si>
+  <si>
+    <t>Sophie's World</t>
+  </si>
+  <si>
+    <t>Solaris</t>
+  </si>
+  <si>
+    <t>Fathers and Sons</t>
+  </si>
+  <si>
+    <t>Doctor Zhivago</t>
+  </si>
+  <si>
+    <t>Germinal</t>
+  </si>
+  <si>
+    <t>The Cherry Orchard</t>
+  </si>
+  <si>
+    <t>Foucault's Pendulum</t>
+  </si>
+  <si>
+    <t>If on a Winter's Night a Traveler</t>
+  </si>
+  <si>
+    <t>Eugene Onegin</t>
+  </si>
+  <si>
+    <t>Invisible Cities</t>
+  </si>
+  <si>
+    <t>The House of Spirits</t>
+  </si>
+  <si>
+    <t>The Book of Laughter and Forgetting</t>
+  </si>
+  <si>
+    <t>The Girl Who Played with Fire</t>
+  </si>
+  <si>
+    <t>The Girl Who Kicked the Hornet's Nest</t>
+  </si>
+  <si>
+    <t>Death in Venice</t>
+  </si>
+  <si>
+    <t>b20</t>
+  </si>
+  <si>
+    <t>b21</t>
+  </si>
+  <si>
+    <t>b22</t>
+  </si>
+  <si>
+    <t>b23</t>
+  </si>
+  <si>
+    <t>b24</t>
+  </si>
+  <si>
+    <t>b25</t>
+  </si>
+  <si>
+    <t>b26</t>
+  </si>
+  <si>
+    <t>b27</t>
+  </si>
+  <si>
+    <t>b28</t>
+  </si>
+  <si>
+    <t>b29</t>
+  </si>
+  <si>
+    <t>b30</t>
+  </si>
+  <si>
+    <t>b31</t>
+  </si>
+  <si>
+    <t>b32</t>
+  </si>
+  <si>
+    <t>b33</t>
+  </si>
+  <si>
+    <t>b34</t>
+  </si>
+  <si>
+    <t>b35</t>
+  </si>
+  <si>
+    <t>b36</t>
+  </si>
+  <si>
+    <t>b37</t>
+  </si>
+  <si>
+    <t>b38</t>
+  </si>
+  <si>
+    <t>b39</t>
+  </si>
+  <si>
+    <t>b40</t>
+  </si>
+  <si>
+    <t>b41</t>
+  </si>
+  <si>
+    <t>b42</t>
+  </si>
+  <si>
+    <t>b43</t>
+  </si>
+  <si>
+    <t>b44</t>
+  </si>
+  <si>
+    <t>b45</t>
+  </si>
+  <si>
+    <t>b46</t>
+  </si>
+  <si>
+    <t>b47</t>
+  </si>
+  <si>
+    <t>b48</t>
+  </si>
+  <si>
+    <t>b49</t>
+  </si>
+  <si>
+    <t>b50</t>
+  </si>
+  <si>
+    <t>b51</t>
+  </si>
+  <si>
+    <t>b52</t>
+  </si>
+  <si>
+    <t>Oblomov</t>
+  </si>
+  <si>
+    <t>Zeno's Conscience</t>
+  </si>
+  <si>
+    <t>Veronika Decides to Die</t>
+  </si>
+  <si>
+    <t>Like Water for Chocolate</t>
+  </si>
+  <si>
+    <t>The Year of the Hare</t>
+  </si>
+  <si>
+    <t>Doppler</t>
+  </si>
+  <si>
+    <t>The Baron in the Trees</t>
+  </si>
+  <si>
+    <t>The Hunchback of Notre-Dame</t>
+  </si>
+  <si>
+    <t>The Rings of Saturn</t>
+  </si>
+  <si>
+    <t>Let the Right One In</t>
+  </si>
+  <si>
+    <t>Zorba the Greek</t>
+  </si>
+  <si>
+    <t>Growth of the Soil</t>
+  </si>
+  <si>
+    <t>A Void</t>
+  </si>
+  <si>
+    <t>Sputnik Sweetheart</t>
+  </si>
+  <si>
+    <t>Convenience Store Woman</t>
+  </si>
+  <si>
+    <t>The Vegetarian</t>
+  </si>
+  <si>
+    <t>The God of Small Things</t>
+  </si>
+  <si>
+    <t>The Neverending Story</t>
+  </si>
+  <si>
+    <t>We</t>
+  </si>
+  <si>
+    <t>The Last Temptation of Christ</t>
+  </si>
+  <si>
+    <t>The Man Who Planted Trees</t>
+  </si>
+  <si>
+    <t>A Man Called Ove</t>
+  </si>
+  <si>
+    <t>Embers</t>
+  </si>
+  <si>
+    <t>Purge</t>
+  </si>
+  <si>
+    <t>The Periodic Table</t>
+  </si>
+  <si>
+    <t>The Elegance of the Hedgehog</t>
+  </si>
+  <si>
+    <t>The Man Who Went Up in Smoke</t>
+  </si>
+  <si>
+    <t>We, The Drowned</t>
+  </si>
+  <si>
+    <t>Hunting and Gathering</t>
+  </si>
+  <si>
+    <t>Last Train to Istanbul</t>
+  </si>
+  <si>
+    <t>The Housekeeper + The Professor</t>
+  </si>
+  <si>
+    <t>Death and the Penguin</t>
+  </si>
+  <si>
+    <t>Heart of a Dog</t>
+  </si>
+  <si>
+    <t>To Live</t>
+  </si>
+  <si>
+    <t>Human Acts</t>
+  </si>
+  <si>
+    <t>The Meursault Investigation</t>
+  </si>
+  <si>
+    <t>A General Theory of Oblivion</t>
+  </si>
+  <si>
+    <t>The Story of the Lost Child</t>
+  </si>
+  <si>
+    <t>The Red Notebook</t>
+  </si>
+  <si>
+    <t>Laurus</t>
+  </si>
+  <si>
+    <t>The Story of My Teeth</t>
+  </si>
+  <si>
+    <t>The Readers of Broken Wheel Recommend</t>
+  </si>
+  <si>
+    <t>Signs Preceding the End of the World</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Drive Your Plow Over the Bones of the Dead</t>
+  </si>
+  <si>
+    <t>The Plotters</t>
+  </si>
+  <si>
+    <t>The Nakano Thrift Shop</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/19380</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/485894</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/4934</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9998</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9717</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/2175</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9712</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/656</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/15823480</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/119073</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/538845</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/40881621</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/11275</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/355697</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/18144590</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/88077</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/2429135</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/11989</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/28381</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/40495148</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/11297</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/4929</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/32585</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/10959</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/95558</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/19117</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/130440</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/28407</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/87346</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/17841</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/374233</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/27822</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9809</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9328</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/240976</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/5060378</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/6892870</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/53061</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/254308</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/84737</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/1431</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/6952</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/656876</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/8171094</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9804</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/30597</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/434903</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/943402</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/53639</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/342049</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/28294</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9557</t>
+  </si>
+  <si>
+    <t>The Sailor Who Fell from Grace with the Sea</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/162332</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/38357895</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/25489025</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/9777</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/27712</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/76171</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/8737</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/757438</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/18774964</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/783505</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/7029668</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/427282</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/2967752</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/913882</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/7988467</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/47780</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/18045473</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/3181564</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/152893</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/113205</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/334971</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/30091914</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/25263557</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/23346410</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/25242224</t>
+  </si>
+  <si>
+    <t>My Grandmother Asked Me to Tell You She's Sorry</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/23604559</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/23129712</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/24694092</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/24796231</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/25573977</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/21535546</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/24493750</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/51648276</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/39618887</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/32919876</t>
+  </si>
+  <si>
+    <t>b53</t>
+  </si>
+  <si>
+    <t>b54</t>
+  </si>
+  <si>
+    <t>b55</t>
+  </si>
+  <si>
+    <t>b56</t>
+  </si>
+  <si>
+    <t>b57</t>
+  </si>
+  <si>
+    <t>b58</t>
+  </si>
+  <si>
+    <t>b59</t>
+  </si>
+  <si>
+    <t>b60</t>
+  </si>
+  <si>
+    <t>b61</t>
+  </si>
+  <si>
+    <t>b62</t>
+  </si>
+  <si>
+    <t>b63</t>
+  </si>
+  <si>
+    <t>b64</t>
+  </si>
+  <si>
+    <t>b65</t>
+  </si>
+  <si>
+    <t>b66</t>
+  </si>
+  <si>
+    <t>b67</t>
+  </si>
+  <si>
+    <t>b68</t>
+  </si>
+  <si>
+    <t>b69</t>
+  </si>
+  <si>
+    <t>b70</t>
+  </si>
+  <si>
+    <t>b71</t>
+  </si>
+  <si>
+    <t>b72</t>
+  </si>
+  <si>
+    <t>b73</t>
+  </si>
+  <si>
+    <t>b74</t>
+  </si>
+  <si>
+    <t>b75</t>
+  </si>
+  <si>
+    <t>b76</t>
+  </si>
+  <si>
+    <t>b77</t>
+  </si>
+  <si>
+    <t>b78</t>
+  </si>
+  <si>
+    <t>b79</t>
+  </si>
+  <si>
+    <t>b80</t>
+  </si>
+  <si>
+    <t>b81</t>
+  </si>
+  <si>
+    <t>b82</t>
+  </si>
+  <si>
+    <t>b83</t>
+  </si>
+  <si>
+    <t>b84</t>
+  </si>
+  <si>
+    <t>b85</t>
+  </si>
+  <si>
+    <t>b86</t>
+  </si>
+  <si>
+    <t>b87</t>
+  </si>
+  <si>
+    <t>b88</t>
+  </si>
+  <si>
+    <t>b89</t>
+  </si>
+  <si>
+    <t>b90</t>
+  </si>
+  <si>
+    <t>b91</t>
+  </si>
+  <si>
+    <t>b92</t>
+  </si>
+  <si>
+    <t>b93</t>
+  </si>
+  <si>
+    <t>b94</t>
+  </si>
+  <si>
+    <t>b95</t>
+  </si>
+  <si>
+    <t>b96</t>
+  </si>
+  <si>
+    <t>b97</t>
+  </si>
+  <si>
+    <t>b98</t>
+  </si>
+  <si>
+    <t>b99</t>
+  </si>
+  <si>
+    <t>b100</t>
+  </si>
+  <si>
+    <t>b101</t>
+  </si>
+  <si>
+    <t>b102</t>
+  </si>
+  <si>
+    <t>b103</t>
+  </si>
+  <si>
+    <t>b104</t>
+  </si>
+  <si>
+    <t>b105</t>
+  </si>
+  <si>
+    <t>b106</t>
+  </si>
+  <si>
+    <t>b107</t>
+  </si>
+  <si>
+    <t>b108</t>
+  </si>
+  <si>
+    <t>b109</t>
+  </si>
+  <si>
+    <t>One Day in the Life of Ivan Denisovich</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/17125</t>
+  </si>
+  <si>
+    <t>The Piano Teacher</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/219879</t>
+  </si>
+  <si>
+    <t>The Tin Drum</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/35743</t>
+  </si>
+  <si>
+    <t>Snow Country</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/14028</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/894154</t>
+  </si>
+  <si>
+    <t>Red Sorghum</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/3140</t>
+  </si>
+  <si>
+    <t>The Bridge on the Drina</t>
+  </si>
+  <si>
+    <t>Kristin Lavransdatter</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/6217</t>
+  </si>
+  <si>
+    <t>Independent People</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/77287</t>
+  </si>
+  <si>
+    <t>Against Nature</t>
+  </si>
+  <si>
+    <t>The Emigrants</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/76507</t>
+  </si>
+  <si>
+    <t>Perfume: The Story of a Murderer</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/343</t>
+  </si>
+  <si>
+    <t>The Clown</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/69091</t>
+  </si>
+  <si>
+    <t>Every Man Dies Alone</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/3344411</t>
+  </si>
+  <si>
+    <t>Measuring the World</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/642231</t>
+  </si>
+  <si>
+    <t>Dream Story</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/157409</t>
+  </si>
+  <si>
+    <t>Smilla's Sense of Snow</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/124509</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/6647312</t>
+  </si>
+  <si>
+    <t>The Leopard</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/625094</t>
+  </si>
+  <si>
+    <t>The Tartar Steppe</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/83017</t>
+  </si>
+  <si>
+    <t>Silk</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/61264</t>
+  </si>
+  <si>
+    <t>The Solitude of Prime Numbers</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/6613956</t>
+  </si>
+  <si>
+    <t>b110</t>
+  </si>
+  <si>
+    <t>b111</t>
+  </si>
+  <si>
+    <t>b112</t>
+  </si>
+  <si>
+    <t>b113</t>
+  </si>
+  <si>
+    <t>b114</t>
+  </si>
+  <si>
+    <t>b115</t>
+  </si>
+  <si>
+    <t>b116</t>
+  </si>
+  <si>
+    <t>b117</t>
+  </si>
+  <si>
+    <t>b118</t>
+  </si>
+  <si>
+    <t>b119</t>
+  </si>
+  <si>
+    <t>b120</t>
+  </si>
+  <si>
+    <t>b121</t>
+  </si>
+  <si>
+    <t>b122</t>
+  </si>
+  <si>
+    <t>b123</t>
+  </si>
+  <si>
+    <t>b124</t>
+  </si>
+  <si>
+    <t>b125</t>
+  </si>
+  <si>
+    <t>b126</t>
+  </si>
+  <si>
+    <t>b127</t>
+  </si>
+  <si>
+    <t>b128</t>
+  </si>
+  <si>
+    <t>b129</t>
+  </si>
+  <si>
+    <t>b130</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/10314376</t>
+  </si>
+  <si>
+    <t>The Prague Cemetery</t>
+  </si>
+  <si>
+    <t>Baudolino</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/10507</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/77810</t>
+  </si>
+  <si>
+    <t>The Days of Abandonment</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/244261</t>
+  </si>
+  <si>
+    <t>The Street of Crocodiles</t>
+  </si>
+  <si>
+    <t>Flights</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/36885304</t>
+  </si>
+  <si>
+    <t>The Egyptian</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/26216087</t>
+  </si>
+  <si>
+    <t>Baltasar and Blimunda</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/2530</t>
+  </si>
+  <si>
+    <t>War with the Newts</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/816440</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/40718205</t>
+  </si>
+  <si>
+    <t>The Dinner</t>
+  </si>
+  <si>
+    <t>The Assault</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/88387</t>
+  </si>
+  <si>
+    <t>The Discovery of Heaven</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/88389</t>
+  </si>
+  <si>
+    <t>b131</t>
+  </si>
+  <si>
+    <t>b132</t>
+  </si>
+  <si>
+    <t>b133</t>
+  </si>
+  <si>
+    <t>b134</t>
+  </si>
+  <si>
+    <t>b135</t>
+  </si>
+  <si>
+    <t>b136</t>
+  </si>
+  <si>
+    <t>b137</t>
+  </si>
+  <si>
+    <t>b138</t>
+  </si>
+  <si>
+    <t>b139</t>
+  </si>
+  <si>
+    <t>b140</t>
+  </si>
+  <si>
+    <t>b141</t>
+  </si>
+  <si>
+    <t>Dirty Snow</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/44153</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/18114335</t>
+  </si>
+  <si>
+    <t>Pietr the Latvian</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/497499</t>
+  </si>
+  <si>
+    <t>The Door</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/318335</t>
+  </si>
+  <si>
+    <t>Fatelessness</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/158217</t>
+  </si>
+  <si>
+    <t>Journey by Moonlight</t>
+  </si>
+  <si>
+    <t>The Eighth Life</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/41071389</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/11455485</t>
+  </si>
+  <si>
+    <t>Satantango</t>
+  </si>
+  <si>
+    <t>b142</t>
+  </si>
+  <si>
+    <t>b143</t>
+  </si>
+  <si>
+    <t>b144</t>
+  </si>
+  <si>
+    <t>b145</t>
+  </si>
+  <si>
+    <t>b146</t>
+  </si>
+  <si>
+    <t>b147</t>
+  </si>
+  <si>
+    <t>b148</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/43452825</t>
+  </si>
+  <si>
+    <t>Abigail</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/36217818</t>
+  </si>
+  <si>
+    <t>b149</t>
+  </si>
+  <si>
+    <t>b150</t>
+  </si>
+  <si>
+    <t>Alexander Dumas</t>
+  </si>
+  <si>
+    <t>Miguel de Cervantes Saavedra</t>
+  </si>
+  <si>
+    <t>Voltaire</t>
+  </si>
+  <si>
+    <t>Kobo Abe</t>
+  </si>
+  <si>
+    <t>Milan Kundera</t>
+  </si>
+  <si>
+    <t>Gustave Flaubert</t>
+  </si>
+  <si>
+    <t>Leo Tolstoy</t>
+  </si>
+  <si>
+    <t>Umberto Eco</t>
+  </si>
+  <si>
+    <t>Henryk Sienkiewicz</t>
+  </si>
+  <si>
+    <t>Fernando Pessoa</t>
+  </si>
+  <si>
+    <t>Haruki Murakami</t>
+  </si>
+  <si>
+    <t>Erich Maria Remarque</t>
+  </si>
+  <si>
+    <t>Paulo Coelho</t>
+  </si>
+  <si>
+    <t>Thomas Mann</t>
+  </si>
+  <si>
+    <t>Stieg Larsson</t>
+  </si>
+  <si>
+    <t>Nikolai Gogol</t>
+  </si>
+  <si>
+    <t>Jose Saramago</t>
+  </si>
+  <si>
+    <t>Knut Hamsun</t>
+  </si>
+  <si>
+    <t>Jostein Gaarder</t>
+  </si>
+  <si>
+    <t>Stanislaw Lem</t>
+  </si>
+  <si>
+    <t>Ivan Turgenev</t>
+  </si>
+  <si>
+    <t>Boris Pasternak</t>
+  </si>
+  <si>
+    <t>Emile Zola</t>
+  </si>
+  <si>
+    <t>Anton Chekhov</t>
+  </si>
+  <si>
+    <t>Italo Calvino</t>
+  </si>
+  <si>
+    <t>Alexander Pushkin</t>
+  </si>
+  <si>
+    <t>Isabel Allende</t>
+  </si>
+  <si>
+    <t>Han Kang</t>
+  </si>
+  <si>
+    <t>Ivan Goncharov</t>
+  </si>
+  <si>
+    <t>Italo Svevo</t>
+  </si>
+  <si>
+    <t>Laura Esquivel</t>
+  </si>
+  <si>
+    <t>Arto Paasilinna</t>
+  </si>
+  <si>
+    <t>Erlend Loe</t>
+  </si>
+  <si>
+    <t>Victor Hugo</t>
+  </si>
+  <si>
+    <t>W.G. Sebald</t>
+  </si>
+  <si>
+    <t>John Ajvide Lindqvist</t>
+  </si>
+  <si>
+    <t>Nikos Kazantzakis</t>
+  </si>
+  <si>
+    <t>Georges Perec</t>
+  </si>
+  <si>
+    <t>Yukio Mishima</t>
+  </si>
+  <si>
+    <t>Sayaka Murata</t>
+  </si>
+  <si>
+    <t>Arundhati Roy</t>
+  </si>
+  <si>
+    <t>Michael Ende</t>
+  </si>
+  <si>
+    <t>Yevgeny Zamyatin</t>
+  </si>
+  <si>
+    <t>Jean Giono</t>
+  </si>
+  <si>
+    <t>Fredrik Backman</t>
+  </si>
+  <si>
+    <t>Sandor Marai</t>
+  </si>
+  <si>
+    <t>Sofi Oksanen</t>
+  </si>
+  <si>
+    <t>Primo Levi</t>
+  </si>
+  <si>
+    <t>Muriel Barbery</t>
+  </si>
+  <si>
+    <t>Maj Sjöwall</t>
+  </si>
+  <si>
+    <t>Carsten Jensen</t>
+  </si>
+  <si>
+    <t>Anna Gavalda</t>
+  </si>
+  <si>
+    <t>Ayşe Kulin</t>
+  </si>
+  <si>
+    <t>Yoko Ogawa</t>
+  </si>
+  <si>
+    <t>Andrey Kurkov</t>
+  </si>
+  <si>
+    <t>Yu Hua</t>
+  </si>
+  <si>
+    <t>Kamel Daoud</t>
+  </si>
+  <si>
+    <t>Jose Eduardo Agualusa</t>
+  </si>
+  <si>
+    <t>Elena Ferrante</t>
+  </si>
+  <si>
+    <t>Antoine Laurain</t>
+  </si>
+  <si>
+    <t>Eugene Vodolazkin</t>
+  </si>
+  <si>
+    <t>Valeria Luiselli</t>
+  </si>
+  <si>
+    <t>Katarina Bivald</t>
+  </si>
+  <si>
+    <t>Yuri Herrera</t>
+  </si>
+  <si>
+    <t>Michel Houellebecq</t>
+  </si>
+  <si>
+    <t>Olga Tokarczuk</t>
+  </si>
+  <si>
+    <t>Un - su Kim</t>
+  </si>
+  <si>
+    <t>Hiromi Kawakami</t>
+  </si>
+  <si>
+    <t>Aleksandr Solzhenitsyn</t>
+  </si>
+  <si>
+    <t>Elfriede Jelinek</t>
+  </si>
+  <si>
+    <t>Günter Grass</t>
+  </si>
+  <si>
+    <t>Yasunari Kawabata</t>
+  </si>
+  <si>
+    <t>Mo Yan</t>
+  </si>
+  <si>
+    <t>Ivo Andric</t>
+  </si>
+  <si>
+    <t>Sigrid Undset</t>
+  </si>
+  <si>
+    <t>Halldor Laxness</t>
+  </si>
+  <si>
+    <t>Joris - Karl Huysmans</t>
+  </si>
+  <si>
+    <t>Patrick Süskind</t>
+  </si>
+  <si>
+    <t>Heinrich Böll</t>
+  </si>
+  <si>
+    <t>Hans Fallada</t>
+  </si>
+  <si>
+    <t>Daniel Kehlmann</t>
+  </si>
+  <si>
+    <t>Arthur Schnitzler</t>
+  </si>
+  <si>
+    <t>Peter Hoeg</t>
+  </si>
+  <si>
+    <t>Janne Teller</t>
+  </si>
+  <si>
+    <t>Giuseppe Tomasi di Lampedusa</t>
+  </si>
+  <si>
+    <t>Go Went Gone</t>
+  </si>
+  <si>
+    <t>Dino Buzzati</t>
+  </si>
+  <si>
+    <t>Alessandro Baricco</t>
+  </si>
+  <si>
+    <t>Paolo Giordano</t>
+  </si>
+  <si>
+    <t>Bruno Schulz</t>
+  </si>
+  <si>
+    <t>Mika Waltari</t>
+  </si>
+  <si>
+    <t>Karel Capek</t>
+  </si>
+  <si>
+    <t>Herman Koch</t>
+  </si>
+  <si>
+    <t>Harry Mulisch</t>
+  </si>
+  <si>
+    <t>Georges Simenon</t>
+  </si>
+  <si>
+    <t>Magda Szabo</t>
+  </si>
+  <si>
+    <t>Imre Kertesz</t>
+  </si>
+  <si>
+    <t>Antal Szerb</t>
+  </si>
+  <si>
+    <t>Nino Haratischwili</t>
+  </si>
+  <si>
+    <t>Laszlo Krasznahorkai</t>
+  </si>
+  <si>
+    <t>Jenny Erpenbeck</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/210255</t>
   </si>
 </sst>
 </file>
@@ -653,10 +2126,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -664,8 +2137,8 @@
     <col min="1" max="1" width="10.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="8.7265625" style="2"/>
@@ -1009,6 +2482,1840 @@
       </c>
       <c r="E20" s="2" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B54" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B55" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B56" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B57" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B58" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B59" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B60" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B61" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B62" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B63" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B64" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B65" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B66" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B67" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B68" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B69" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B70" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B71" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B72" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B73" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B74" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B75" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B76" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B77" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B78" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B79" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B80" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B81" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B82" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B83" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B84" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B85" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B86" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B87" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B88" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B89" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B90" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B91" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B92" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B93" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B94" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B95" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B96" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B97" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B98" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B99" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B100" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B101" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B102" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="103" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B103" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B104" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B105" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="106" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B106" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B107" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B108" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B109" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B110" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B111" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B112" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B114" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B115" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B119" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B120" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B121" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B122" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B124" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B125" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B126" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B127" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="128" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B128" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B130" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B132" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B134" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B135" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B136" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B137" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B138" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B139" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B140" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B141" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B142" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B143" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B144" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="D145" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B149" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B150" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B151" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D151" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>
@@ -1032,8 +4339,47 @@
     <hyperlink ref="B18" r:id="rId16" xr:uid="{6137B346-D334-4B5F-BA68-74835140C59F}"/>
     <hyperlink ref="B19" r:id="rId17" xr:uid="{0350EED7-0846-4FDE-AC88-8F2E79513C0A}"/>
     <hyperlink ref="B20" r:id="rId18" xr:uid="{22BAC466-A4DE-494E-91D7-4653EB0FFDE8}"/>
+    <hyperlink ref="B21" r:id="rId19" xr:uid="{C91AF671-19DC-42F3-8941-C5B4E197FA43}"/>
+    <hyperlink ref="B30" r:id="rId20" xr:uid="{40C71865-CAE4-4C90-90EB-C95684C7C659}"/>
+    <hyperlink ref="B36" r:id="rId21" xr:uid="{E2D964BD-C4A8-4C71-9F3C-0D6758882C3E}"/>
+    <hyperlink ref="B37" r:id="rId22" xr:uid="{A11967DA-E17E-45B4-B152-7BC8E731EC4E}"/>
+    <hyperlink ref="B54" r:id="rId23" xr:uid="{94208E05-4C81-44EC-9F0D-A856858AFA75}"/>
+    <hyperlink ref="B55" r:id="rId24" xr:uid="{854B2FFB-98CA-49B3-95FA-C42DBFCD1EF7}"/>
+    <hyperlink ref="B56" r:id="rId25" xr:uid="{B9DC23E7-ED6C-4B36-9819-6454FE8524E5}"/>
+    <hyperlink ref="B57" r:id="rId26" xr:uid="{002207AC-3631-4FB7-B8BB-E371E15D41C9}"/>
+    <hyperlink ref="B58" r:id="rId27" xr:uid="{0648CE20-BA35-4EA9-AA34-73289382D179}"/>
+    <hyperlink ref="B59" r:id="rId28" xr:uid="{BDAA86B3-6146-4394-8DB0-EBA4AFD625F1}"/>
+    <hyperlink ref="B63" r:id="rId29" xr:uid="{3556CC4A-3DBC-4274-8040-447BDEC0483B}"/>
+    <hyperlink ref="B60" r:id="rId30" xr:uid="{A8141101-8CA8-43CA-A838-4976D1F61937}"/>
+    <hyperlink ref="B61" r:id="rId31" xr:uid="{2050D124-EB58-428A-8825-C025C0A23BCE}"/>
+    <hyperlink ref="B62" r:id="rId32" xr:uid="{AC76B35A-C8D1-4A3A-9C3F-B24F2D5A8620}"/>
+    <hyperlink ref="B64" r:id="rId33" xr:uid="{B59F6412-F36C-4B21-B694-198B24F53B27}"/>
+    <hyperlink ref="B65" r:id="rId34" xr:uid="{B1C601ED-5C15-404E-8582-7E4ABA8783F8}"/>
+    <hyperlink ref="B66" r:id="rId35" xr:uid="{6E9B2687-EFEF-4FCB-91FB-662C839564F6}"/>
+    <hyperlink ref="B67" r:id="rId36" xr:uid="{D08186DE-CA7B-41D4-A96F-7FC1D10B39E1}"/>
+    <hyperlink ref="B68" r:id="rId37" xr:uid="{51D5B3E5-0AB6-4875-A76D-60D9753D4F86}"/>
+    <hyperlink ref="B69" r:id="rId38" xr:uid="{5FBB9C03-0804-454E-BA87-43AD2928C3B0}"/>
+    <hyperlink ref="B70" r:id="rId39" xr:uid="{611C3710-9207-4AEC-BBA1-E523C7FC1110}"/>
+    <hyperlink ref="B71" r:id="rId40" xr:uid="{47138D79-BA74-4DB4-A20A-CDD7125D3BAE}"/>
+    <hyperlink ref="B72" r:id="rId41" xr:uid="{E6E80776-D6D4-43F8-A33E-003185FD9513}"/>
+    <hyperlink ref="B73" r:id="rId42" xr:uid="{213BD1D7-1EA2-421A-B8AD-1F1E947CB611}"/>
+    <hyperlink ref="B74" r:id="rId43" xr:uid="{C4B03A82-408C-476F-B243-406A29DD9714}"/>
+    <hyperlink ref="B75" r:id="rId44" xr:uid="{5F2DE561-C8C3-4469-94CE-EA557B32555D}"/>
+    <hyperlink ref="B76" r:id="rId45" xr:uid="{782E1633-963D-4CE0-A16A-5A98C5D74C5F}"/>
+    <hyperlink ref="B77" r:id="rId46" xr:uid="{AE65DEF7-1885-47C6-AA1E-EB808C9E3C81}"/>
+    <hyperlink ref="B78" r:id="rId47" xr:uid="{8982E8D0-459F-44FC-9D86-2AED83A2573F}"/>
+    <hyperlink ref="B79" r:id="rId48" xr:uid="{F8537249-1CDF-494F-9D1A-891D8A6F0E2F}"/>
+    <hyperlink ref="B80" r:id="rId49" xr:uid="{486D425A-598E-4F3A-89BD-8EB8C9D7B327}"/>
+    <hyperlink ref="B81" r:id="rId50" xr:uid="{3EAFCC59-29F0-44F5-B7A1-6E126E4EA0AB}"/>
+    <hyperlink ref="B82" r:id="rId51" xr:uid="{73A94274-5959-4EBD-A21B-A39D6292EE49}"/>
+    <hyperlink ref="B84" r:id="rId52" xr:uid="{6B53746B-9333-4DA3-B799-0B460626AE1E}"/>
+    <hyperlink ref="B86" r:id="rId53" xr:uid="{95FAAF25-68C5-4D4B-8B52-022DBF4B3397}"/>
+    <hyperlink ref="B96" r:id="rId54" xr:uid="{E053E535-0383-475F-8194-BAAAD8D1A211}"/>
+    <hyperlink ref="B114" r:id="rId55" xr:uid="{93FA574D-996B-4125-A0D5-16EFC2012875}"/>
+    <hyperlink ref="B128" r:id="rId56" xr:uid="{1ADD84E1-B71D-4B73-97D0-4E07A135A680}"/>
+    <hyperlink ref="B119" r:id="rId57" xr:uid="{F6A76550-879F-463B-8337-25D90C642687}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor changes to book_data_external.xlsx
</commit_message>
<xml_diff>
--- a/data/external/book_data_external.xlsx
+++ b/data/external/book_data_external.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejgen\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\Study Documents\School\Bachelor's Paper - Seeking Traces of the Translator's Invisibility in Goodreads Reviews\Code\bachelors_paper_proof_of_concept\data\external\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80197CBA-22BD-4B63-BC48-A43DADC9BE4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285ED1E9-B26C-47D2-BC17-B2DA1E2D78FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="60" windowWidth="19180" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="713">
   <si>
     <t>http</t>
   </si>
@@ -1771,6 +1771,399 @@
   </si>
   <si>
     <t>https://www.goodreads.com/book/show/210255</t>
+  </si>
+  <si>
+    <t>h20</t>
+  </si>
+  <si>
+    <t>h21</t>
+  </si>
+  <si>
+    <t>h22</t>
+  </si>
+  <si>
+    <t>h23</t>
+  </si>
+  <si>
+    <t>h24</t>
+  </si>
+  <si>
+    <t>h25</t>
+  </si>
+  <si>
+    <t>h26</t>
+  </si>
+  <si>
+    <t>h27</t>
+  </si>
+  <si>
+    <t>h28</t>
+  </si>
+  <si>
+    <t>h29</t>
+  </si>
+  <si>
+    <t>h30</t>
+  </si>
+  <si>
+    <t>h31</t>
+  </si>
+  <si>
+    <t>h32</t>
+  </si>
+  <si>
+    <t>h33</t>
+  </si>
+  <si>
+    <t>h34</t>
+  </si>
+  <si>
+    <t>h35</t>
+  </si>
+  <si>
+    <t>h36</t>
+  </si>
+  <si>
+    <t>h37</t>
+  </si>
+  <si>
+    <t>h38</t>
+  </si>
+  <si>
+    <t>h39</t>
+  </si>
+  <si>
+    <t>h40</t>
+  </si>
+  <si>
+    <t>h41</t>
+  </si>
+  <si>
+    <t>h42</t>
+  </si>
+  <si>
+    <t>h43</t>
+  </si>
+  <si>
+    <t>h44</t>
+  </si>
+  <si>
+    <t>h45</t>
+  </si>
+  <si>
+    <t>h46</t>
+  </si>
+  <si>
+    <t>h47</t>
+  </si>
+  <si>
+    <t>h48</t>
+  </si>
+  <si>
+    <t>h49</t>
+  </si>
+  <si>
+    <t>h50</t>
+  </si>
+  <si>
+    <t>h51</t>
+  </si>
+  <si>
+    <t>h52</t>
+  </si>
+  <si>
+    <t>h53</t>
+  </si>
+  <si>
+    <t>h54</t>
+  </si>
+  <si>
+    <t>h55</t>
+  </si>
+  <si>
+    <t>h56</t>
+  </si>
+  <si>
+    <t>h57</t>
+  </si>
+  <si>
+    <t>h58</t>
+  </si>
+  <si>
+    <t>h59</t>
+  </si>
+  <si>
+    <t>h60</t>
+  </si>
+  <si>
+    <t>h61</t>
+  </si>
+  <si>
+    <t>h62</t>
+  </si>
+  <si>
+    <t>h63</t>
+  </si>
+  <si>
+    <t>h64</t>
+  </si>
+  <si>
+    <t>h65</t>
+  </si>
+  <si>
+    <t>h66</t>
+  </si>
+  <si>
+    <t>h67</t>
+  </si>
+  <si>
+    <t>h68</t>
+  </si>
+  <si>
+    <t>h69</t>
+  </si>
+  <si>
+    <t>h70</t>
+  </si>
+  <si>
+    <t>h71</t>
+  </si>
+  <si>
+    <t>h72</t>
+  </si>
+  <si>
+    <t>h73</t>
+  </si>
+  <si>
+    <t>h74</t>
+  </si>
+  <si>
+    <t>h75</t>
+  </si>
+  <si>
+    <t>h76</t>
+  </si>
+  <si>
+    <t>h77</t>
+  </si>
+  <si>
+    <t>h78</t>
+  </si>
+  <si>
+    <t>h79</t>
+  </si>
+  <si>
+    <t>h80</t>
+  </si>
+  <si>
+    <t>h81</t>
+  </si>
+  <si>
+    <t>h82</t>
+  </si>
+  <si>
+    <t>h83</t>
+  </si>
+  <si>
+    <t>h84</t>
+  </si>
+  <si>
+    <t>h85</t>
+  </si>
+  <si>
+    <t>h86</t>
+  </si>
+  <si>
+    <t>h87</t>
+  </si>
+  <si>
+    <t>h88</t>
+  </si>
+  <si>
+    <t>h89</t>
+  </si>
+  <si>
+    <t>h90</t>
+  </si>
+  <si>
+    <t>h91</t>
+  </si>
+  <si>
+    <t>h92</t>
+  </si>
+  <si>
+    <t>h93</t>
+  </si>
+  <si>
+    <t>h94</t>
+  </si>
+  <si>
+    <t>h95</t>
+  </si>
+  <si>
+    <t>h96</t>
+  </si>
+  <si>
+    <t>h97</t>
+  </si>
+  <si>
+    <t>h98</t>
+  </si>
+  <si>
+    <t>h99</t>
+  </si>
+  <si>
+    <t>h100</t>
+  </si>
+  <si>
+    <t>h101</t>
+  </si>
+  <si>
+    <t>h102</t>
+  </si>
+  <si>
+    <t>h103</t>
+  </si>
+  <si>
+    <t>h104</t>
+  </si>
+  <si>
+    <t>h105</t>
+  </si>
+  <si>
+    <t>h106</t>
+  </si>
+  <si>
+    <t>h107</t>
+  </si>
+  <si>
+    <t>h108</t>
+  </si>
+  <si>
+    <t>h109</t>
+  </si>
+  <si>
+    <t>h110</t>
+  </si>
+  <si>
+    <t>h111</t>
+  </si>
+  <si>
+    <t>h112</t>
+  </si>
+  <si>
+    <t>h113</t>
+  </si>
+  <si>
+    <t>h114</t>
+  </si>
+  <si>
+    <t>h115</t>
+  </si>
+  <si>
+    <t>h116</t>
+  </si>
+  <si>
+    <t>h117</t>
+  </si>
+  <si>
+    <t>h118</t>
+  </si>
+  <si>
+    <t>h119</t>
+  </si>
+  <si>
+    <t>h120</t>
+  </si>
+  <si>
+    <t>h121</t>
+  </si>
+  <si>
+    <t>h122</t>
+  </si>
+  <si>
+    <t>h123</t>
+  </si>
+  <si>
+    <t>h124</t>
+  </si>
+  <si>
+    <t>h125</t>
+  </si>
+  <si>
+    <t>h126</t>
+  </si>
+  <si>
+    <t>h127</t>
+  </si>
+  <si>
+    <t>h128</t>
+  </si>
+  <si>
+    <t>h129</t>
+  </si>
+  <si>
+    <t>h130</t>
+  </si>
+  <si>
+    <t>h131</t>
+  </si>
+  <si>
+    <t>h132</t>
+  </si>
+  <si>
+    <t>h133</t>
+  </si>
+  <si>
+    <t>h134</t>
+  </si>
+  <si>
+    <t>h135</t>
+  </si>
+  <si>
+    <t>h136</t>
+  </si>
+  <si>
+    <t>h137</t>
+  </si>
+  <si>
+    <t>h138</t>
+  </si>
+  <si>
+    <t>h139</t>
+  </si>
+  <si>
+    <t>h140</t>
+  </si>
+  <si>
+    <t>h141</t>
+  </si>
+  <si>
+    <t>h142</t>
+  </si>
+  <si>
+    <t>h143</t>
+  </si>
+  <si>
+    <t>h144</t>
+  </si>
+  <si>
+    <t>h145</t>
+  </si>
+  <si>
+    <t>h146</t>
+  </si>
+  <si>
+    <t>h147</t>
+  </si>
+  <si>
+    <t>h148</t>
+  </si>
+  <si>
+    <t>h149</t>
+  </si>
+  <si>
+    <t>h150</t>
   </si>
 </sst>
 </file>
@@ -2128,8 +2521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2485,6 +2878,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>582</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>92</v>
       </c>
@@ -2499,6 +2895,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>583</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>94</v>
       </c>
@@ -2513,6 +2912,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>584</v>
+      </c>
       <c r="B23" s="2" t="s">
         <v>213</v>
       </c>
@@ -2527,6 +2929,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>585</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>214</v>
       </c>
@@ -2541,6 +2946,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>586</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>215</v>
       </c>
@@ -2555,6 +2963,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>587</v>
+      </c>
       <c r="B26" s="2" t="s">
         <v>216</v>
       </c>
@@ -2569,6 +2980,9 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>588</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>217</v>
       </c>
@@ -2583,6 +2997,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>589</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>218</v>
       </c>
@@ -2597,6 +3014,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>590</v>
+      </c>
       <c r="B29" s="2" t="s">
         <v>219</v>
       </c>
@@ -2611,6 +3031,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>591</v>
+      </c>
       <c r="B30" s="1" t="s">
         <v>220</v>
       </c>
@@ -2625,6 +3048,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>592</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>221</v>
       </c>
@@ -2639,6 +3065,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>593</v>
+      </c>
       <c r="B32" s="2" t="s">
         <v>222</v>
       </c>
@@ -2652,7 +3081,10 @@
         <v>487</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>594</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>223</v>
       </c>
@@ -2666,7 +3098,10 @@
         <v>488</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>595</v>
+      </c>
       <c r="B34" s="2" t="s">
         <v>224</v>
       </c>
@@ -2680,7 +3115,10 @@
         <v>489</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>596</v>
+      </c>
       <c r="B35" s="2" t="s">
         <v>225</v>
       </c>
@@ -2694,7 +3132,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3" t="s">
+        <v>597</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>226</v>
       </c>
@@ -2708,7 +3149,10 @@
         <v>491</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>598</v>
+      </c>
       <c r="B37" s="1" t="s">
         <v>227</v>
       </c>
@@ -2722,7 +3166,10 @@
         <v>492</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>599</v>
+      </c>
       <c r="B38" s="2" t="s">
         <v>228</v>
       </c>
@@ -2736,7 +3183,10 @@
         <v>493</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>600</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>229</v>
       </c>
@@ -2750,7 +3200,10 @@
         <v>494</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>601</v>
+      </c>
       <c r="B40" s="2" t="s">
         <v>230</v>
       </c>
@@ -2764,7 +3217,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>602</v>
+      </c>
       <c r="B41" s="2" t="s">
         <v>231</v>
       </c>
@@ -2778,7 +3234,10 @@
         <v>495</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>603</v>
+      </c>
       <c r="B42" s="2" t="s">
         <v>232</v>
       </c>
@@ -2792,7 +3251,10 @@
         <v>496</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>604</v>
+      </c>
       <c r="B43" s="2" t="s">
         <v>233</v>
       </c>
@@ -2806,7 +3268,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>605</v>
+      </c>
       <c r="B44" s="2" t="s">
         <v>234</v>
       </c>
@@ -2820,7 +3285,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>606</v>
+      </c>
       <c r="B45" s="2" t="s">
         <v>235</v>
       </c>
@@ -2834,7 +3302,10 @@
         <v>497</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>607</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>236</v>
       </c>
@@ -2848,7 +3319,10 @@
         <v>498</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>608</v>
+      </c>
       <c r="B47" s="2" t="s">
         <v>237</v>
       </c>
@@ -2862,7 +3336,10 @@
         <v>499</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>609</v>
+      </c>
       <c r="B48" s="2" t="s">
         <v>238</v>
       </c>
@@ -2876,7 +3353,10 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>610</v>
+      </c>
       <c r="B49" s="2" t="s">
         <v>239</v>
       </c>
@@ -2890,7 +3370,10 @@
         <v>501</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>611</v>
+      </c>
       <c r="B50" s="2" t="s">
         <v>240</v>
       </c>
@@ -2904,7 +3387,10 @@
         <v>502</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>612</v>
+      </c>
       <c r="B51" s="2" t="s">
         <v>241</v>
       </c>
@@ -2918,7 +3404,10 @@
         <v>503</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>613</v>
+      </c>
       <c r="B52" s="2" t="s">
         <v>242</v>
       </c>
@@ -2932,7 +3421,10 @@
         <v>487</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>614</v>
+      </c>
       <c r="B53" s="2" t="s">
         <v>243</v>
       </c>
@@ -2946,7 +3438,10 @@
         <v>504</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="3" t="s">
+        <v>615</v>
+      </c>
       <c r="B54" s="1" t="s">
         <v>244</v>
       </c>
@@ -2960,7 +3455,10 @@
         <v>505</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="B55" s="1" t="s">
         <v>245</v>
       </c>
@@ -2974,7 +3472,10 @@
         <v>504</v>
       </c>
     </row>
-    <row r="56" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A56" s="3" t="s">
+        <v>617</v>
+      </c>
       <c r="B56" s="1" t="s">
         <v>246</v>
       </c>
@@ -2988,7 +3489,10 @@
         <v>506</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>618</v>
+      </c>
       <c r="B57" s="1" t="s">
         <v>247</v>
       </c>
@@ -3002,7 +3506,10 @@
         <v>484</v>
       </c>
     </row>
-    <row r="58" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>619</v>
+      </c>
       <c r="B58" s="1" t="s">
         <v>248</v>
       </c>
@@ -3016,7 +3523,10 @@
         <v>494</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>620</v>
+      </c>
       <c r="B59" s="1" t="s">
         <v>249</v>
       </c>
@@ -3030,7 +3540,10 @@
         <v>494</v>
       </c>
     </row>
-    <row r="60" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A60" s="3" t="s">
+        <v>621</v>
+      </c>
       <c r="B60" s="1" t="s">
         <v>250</v>
       </c>
@@ -3044,7 +3557,10 @@
         <v>493</v>
       </c>
     </row>
-    <row r="61" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>622</v>
+      </c>
       <c r="B61" s="1" t="s">
         <v>251</v>
       </c>
@@ -3058,7 +3574,10 @@
         <v>508</v>
       </c>
     </row>
-    <row r="62" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>623</v>
+      </c>
       <c r="B62" s="1" t="s">
         <v>252</v>
       </c>
@@ -3072,7 +3591,10 @@
         <v>509</v>
       </c>
     </row>
-    <row r="63" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A63" s="3" t="s">
+        <v>624</v>
+      </c>
       <c r="B63" s="1" t="s">
         <v>253</v>
       </c>
@@ -3086,7 +3608,10 @@
         <v>492</v>
       </c>
     </row>
-    <row r="64" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A64" s="3" t="s">
+        <v>625</v>
+      </c>
       <c r="B64" s="1" t="s">
         <v>254</v>
       </c>
@@ -3100,7 +3625,10 @@
         <v>510</v>
       </c>
     </row>
-    <row r="65" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="3" t="s">
+        <v>626</v>
+      </c>
       <c r="B65" s="1" t="s">
         <v>255</v>
       </c>
@@ -3114,7 +3642,10 @@
         <v>511</v>
       </c>
     </row>
-    <row r="66" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A66" s="3" t="s">
+        <v>627</v>
+      </c>
       <c r="B66" s="1" t="s">
         <v>256</v>
       </c>
@@ -3128,7 +3659,10 @@
         <v>512</v>
       </c>
     </row>
-    <row r="67" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="3" t="s">
+        <v>628</v>
+      </c>
       <c r="B67" s="1" t="s">
         <v>257</v>
       </c>
@@ -3142,7 +3676,10 @@
         <v>504</v>
       </c>
     </row>
-    <row r="68" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>629</v>
+      </c>
       <c r="B68" s="1" t="s">
         <v>258</v>
       </c>
@@ -3156,7 +3693,10 @@
         <v>513</v>
       </c>
     </row>
-    <row r="69" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>630</v>
+      </c>
       <c r="B69" s="1" t="s">
         <v>259</v>
       </c>
@@ -3170,7 +3710,10 @@
         <v>514</v>
       </c>
     </row>
-    <row r="70" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>631</v>
+      </c>
       <c r="B70" s="1" t="s">
         <v>260</v>
       </c>
@@ -3184,7 +3727,10 @@
         <v>515</v>
       </c>
     </row>
-    <row r="71" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="3" t="s">
+        <v>632</v>
+      </c>
       <c r="B71" s="1" t="s">
         <v>261</v>
       </c>
@@ -3198,7 +3744,10 @@
         <v>516</v>
       </c>
     </row>
-    <row r="72" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A72" s="3" t="s">
+        <v>633</v>
+      </c>
       <c r="B72" s="1" t="s">
         <v>262</v>
       </c>
@@ -3212,7 +3761,10 @@
         <v>497</v>
       </c>
     </row>
-    <row r="73" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="3" t="s">
+        <v>634</v>
+      </c>
       <c r="B73" s="1" t="s">
         <v>263</v>
       </c>
@@ -3226,7 +3778,10 @@
         <v>517</v>
       </c>
     </row>
-    <row r="74" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>635</v>
+      </c>
       <c r="B74" s="1" t="s">
         <v>264</v>
       </c>
@@ -3240,7 +3795,10 @@
         <v>490</v>
       </c>
     </row>
-    <row r="75" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A75" s="3" t="s">
+        <v>636</v>
+      </c>
       <c r="B75" s="1" t="s">
         <v>266</v>
       </c>
@@ -3254,7 +3812,10 @@
         <v>518</v>
       </c>
     </row>
-    <row r="76" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A76" s="3" t="s">
+        <v>637</v>
+      </c>
       <c r="B76" s="1" t="s">
         <v>267</v>
       </c>
@@ -3268,7 +3829,10 @@
         <v>519</v>
       </c>
     </row>
-    <row r="77" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A77" s="3" t="s">
+        <v>638</v>
+      </c>
       <c r="B77" s="1" t="s">
         <v>268</v>
       </c>
@@ -3282,7 +3846,10 @@
         <v>507</v>
       </c>
     </row>
-    <row r="78" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
+        <v>639</v>
+      </c>
       <c r="B78" s="1" t="s">
         <v>269</v>
       </c>
@@ -3296,7 +3863,10 @@
         <v>520</v>
       </c>
     </row>
-    <row r="79" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A79" s="3" t="s">
+        <v>640</v>
+      </c>
       <c r="B79" s="1" t="s">
         <v>270</v>
       </c>
@@ -3310,7 +3880,10 @@
         <v>521</v>
       </c>
     </row>
-    <row r="80" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
+        <v>641</v>
+      </c>
       <c r="B80" s="1" t="s">
         <v>271</v>
       </c>
@@ -3324,7 +3897,10 @@
         <v>522</v>
       </c>
     </row>
-    <row r="81" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A81" s="3" t="s">
+        <v>642</v>
+      </c>
       <c r="B81" s="1" t="s">
         <v>272</v>
       </c>
@@ -3338,7 +3914,10 @@
         <v>516</v>
       </c>
     </row>
-    <row r="82" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A82" s="3" t="s">
+        <v>643</v>
+      </c>
       <c r="B82" s="1" t="s">
         <v>273</v>
       </c>
@@ -3352,7 +3931,10 @@
         <v>523</v>
       </c>
     </row>
-    <row r="83" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A83" s="3" t="s">
+        <v>644</v>
+      </c>
       <c r="B83" s="1" t="s">
         <v>274</v>
       </c>
@@ -3366,7 +3948,10 @@
         <v>524</v>
       </c>
     </row>
-    <row r="84" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A84" s="3" t="s">
+        <v>645</v>
+      </c>
       <c r="B84" s="1" t="s">
         <v>275</v>
       </c>
@@ -3380,7 +3965,10 @@
         <v>525</v>
       </c>
     </row>
-    <row r="85" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A85" s="3" t="s">
+        <v>646</v>
+      </c>
       <c r="B85" s="1" t="s">
         <v>276</v>
       </c>
@@ -3394,7 +3982,10 @@
         <v>526</v>
       </c>
     </row>
-    <row r="86" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A86" s="3" t="s">
+        <v>647</v>
+      </c>
       <c r="B86" s="1" t="s">
         <v>277</v>
       </c>
@@ -3408,7 +3999,10 @@
         <v>527</v>
       </c>
     </row>
-    <row r="87" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A87" s="3" t="s">
+        <v>648</v>
+      </c>
       <c r="B87" s="1" t="s">
         <v>278</v>
       </c>
@@ -3422,7 +4016,10 @@
         <v>528</v>
       </c>
     </row>
-    <row r="88" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A88" s="3" t="s">
+        <v>649</v>
+      </c>
       <c r="B88" s="1" t="s">
         <v>279</v>
       </c>
@@ -3436,7 +4033,10 @@
         <v>529</v>
       </c>
     </row>
-    <row r="89" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A89" s="3" t="s">
+        <v>650</v>
+      </c>
       <c r="B89" s="1" t="s">
         <v>280</v>
       </c>
@@ -3450,7 +4050,10 @@
         <v>530</v>
       </c>
     </row>
-    <row r="90" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>651</v>
+      </c>
       <c r="B90" s="1" t="s">
         <v>281</v>
       </c>
@@ -3464,7 +4067,10 @@
         <v>531</v>
       </c>
     </row>
-    <row r="91" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>652</v>
+      </c>
       <c r="B91" s="1" t="s">
         <v>282</v>
       </c>
@@ -3478,7 +4084,10 @@
         <v>532</v>
       </c>
     </row>
-    <row r="92" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A92" s="3" t="s">
+        <v>653</v>
+      </c>
       <c r="B92" s="1" t="s">
         <v>283</v>
       </c>
@@ -3492,7 +4101,10 @@
         <v>533</v>
       </c>
     </row>
-    <row r="93" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A93" s="3" t="s">
+        <v>654</v>
+      </c>
       <c r="B93" s="1" t="s">
         <v>58</v>
       </c>
@@ -3506,7 +4118,10 @@
         <v>57</v>
       </c>
     </row>
-    <row r="94" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
+        <v>655</v>
+      </c>
       <c r="B94" s="1" t="s">
         <v>284</v>
       </c>
@@ -3520,7 +4135,10 @@
         <v>534</v>
       </c>
     </row>
-    <row r="95" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A95" s="3" t="s">
+        <v>656</v>
+      </c>
       <c r="B95" s="1" t="s">
         <v>285</v>
       </c>
@@ -3534,7 +4152,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A96" s="3" t="s">
+        <v>657</v>
+      </c>
       <c r="B96" s="1" t="s">
         <v>286</v>
       </c>
@@ -3548,7 +4169,10 @@
         <v>535</v>
       </c>
     </row>
-    <row r="97" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A97" s="3" t="s">
+        <v>658</v>
+      </c>
       <c r="B97" s="1" t="s">
         <v>287</v>
       </c>
@@ -3562,7 +4186,10 @@
         <v>507</v>
       </c>
     </row>
-    <row r="98" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A98" s="3" t="s">
+        <v>659</v>
+      </c>
       <c r="B98" s="1" t="s">
         <v>288</v>
       </c>
@@ -3576,7 +4203,10 @@
         <v>536</v>
       </c>
     </row>
-    <row r="99" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A99" s="3" t="s">
+        <v>660</v>
+      </c>
       <c r="B99" s="1" t="s">
         <v>289</v>
       </c>
@@ -3590,7 +4220,10 @@
         <v>537</v>
       </c>
     </row>
-    <row r="100" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A100" s="3" t="s">
+        <v>661</v>
+      </c>
       <c r="B100" s="1" t="s">
         <v>290</v>
       </c>
@@ -3604,7 +4237,10 @@
         <v>538</v>
       </c>
     </row>
-    <row r="101" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A101" s="3" t="s">
+        <v>662</v>
+      </c>
       <c r="B101" s="1" t="s">
         <v>292</v>
       </c>
@@ -3618,7 +4254,10 @@
         <v>524</v>
       </c>
     </row>
-    <row r="102" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>663</v>
+      </c>
       <c r="B102" s="1" t="s">
         <v>293</v>
       </c>
@@ -3632,7 +4271,10 @@
         <v>539</v>
       </c>
     </row>
-    <row r="103" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A103" s="3" t="s">
+        <v>664</v>
+      </c>
       <c r="B103" s="1" t="s">
         <v>294</v>
       </c>
@@ -3646,7 +4288,10 @@
         <v>540</v>
       </c>
     </row>
-    <row r="104" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A104" s="3" t="s">
+        <v>665</v>
+      </c>
       <c r="B104" s="1" t="s">
         <v>295</v>
       </c>
@@ -3660,7 +4305,10 @@
         <v>541</v>
       </c>
     </row>
-    <row r="105" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A105" s="3" t="s">
+        <v>666</v>
+      </c>
       <c r="B105" s="1" t="s">
         <v>296</v>
       </c>
@@ -3674,7 +4322,10 @@
         <v>542</v>
       </c>
     </row>
-    <row r="106" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A106" s="3" t="s">
+        <v>667</v>
+      </c>
       <c r="B106" s="1" t="s">
         <v>297</v>
       </c>
@@ -3688,7 +4339,10 @@
         <v>543</v>
       </c>
     </row>
-    <row r="107" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="3" t="s">
+        <v>668</v>
+      </c>
       <c r="B107" s="1" t="s">
         <v>298</v>
       </c>
@@ -3702,7 +4356,10 @@
         <v>544</v>
       </c>
     </row>
-    <row r="108" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A108" s="3" t="s">
+        <v>669</v>
+      </c>
       <c r="B108" s="1" t="s">
         <v>299</v>
       </c>
@@ -3716,7 +4373,10 @@
         <v>545</v>
       </c>
     </row>
-    <row r="109" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A109" s="3" t="s">
+        <v>670</v>
+      </c>
       <c r="B109" s="1" t="s">
         <v>300</v>
       </c>
@@ -3730,7 +4390,10 @@
         <v>546</v>
       </c>
     </row>
-    <row r="110" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A110" s="3" t="s">
+        <v>671</v>
+      </c>
       <c r="B110" s="1" t="s">
         <v>301</v>
       </c>
@@ -3744,7 +4407,10 @@
         <v>547</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>672</v>
+      </c>
       <c r="B111" s="2" t="s">
         <v>360</v>
       </c>
@@ -3758,7 +4424,10 @@
         <v>548</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>673</v>
+      </c>
       <c r="B112" s="2" t="s">
         <v>362</v>
       </c>
@@ -3772,7 +4441,10 @@
         <v>549</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>674</v>
+      </c>
       <c r="B113" s="2" t="s">
         <v>364</v>
       </c>
@@ -3786,7 +4458,10 @@
         <v>550</v>
       </c>
     </row>
-    <row r="114" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A114" s="3" t="s">
+        <v>675</v>
+      </c>
       <c r="B114" s="1" t="s">
         <v>366</v>
       </c>
@@ -3800,7 +4475,10 @@
         <v>551</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>676</v>
+      </c>
       <c r="B115" s="2" t="s">
         <v>367</v>
       </c>
@@ -3814,7 +4492,10 @@
         <v>552</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>677</v>
+      </c>
       <c r="B116" s="2" t="s">
         <v>369</v>
       </c>
@@ -3828,7 +4509,10 @@
         <v>553</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>678</v>
+      </c>
       <c r="B117" s="2" t="s">
         <v>372</v>
       </c>
@@ -3842,7 +4526,10 @@
         <v>554</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>679</v>
+      </c>
       <c r="B118" s="2" t="s">
         <v>374</v>
       </c>
@@ -3856,7 +4543,10 @@
         <v>555</v>
       </c>
     </row>
-    <row r="119" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A119" s="3" t="s">
+        <v>680</v>
+      </c>
       <c r="B119" s="1" t="s">
         <v>581</v>
       </c>
@@ -3870,7 +4560,10 @@
         <v>556</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>681</v>
+      </c>
       <c r="B120" s="2" t="s">
         <v>377</v>
       </c>
@@ -3884,7 +4577,10 @@
         <v>514</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>682</v>
+      </c>
       <c r="B121" s="2" t="s">
         <v>379</v>
       </c>
@@ -3898,7 +4594,10 @@
         <v>557</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>683</v>
+      </c>
       <c r="B122" s="2" t="s">
         <v>381</v>
       </c>
@@ -3912,7 +4611,10 @@
         <v>558</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>684</v>
+      </c>
       <c r="B123" s="2" t="s">
         <v>383</v>
       </c>
@@ -3926,7 +4628,10 @@
         <v>559</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>685</v>
+      </c>
       <c r="B124" s="2" t="s">
         <v>385</v>
       </c>
@@ -3940,7 +4645,10 @@
         <v>560</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>686</v>
+      </c>
       <c r="B125" s="2" t="s">
         <v>387</v>
       </c>
@@ -3954,7 +4662,10 @@
         <v>561</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>687</v>
+      </c>
       <c r="B126" s="2" t="s">
         <v>389</v>
       </c>
@@ -3968,7 +4679,10 @@
         <v>562</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>688</v>
+      </c>
       <c r="B127" s="2" t="s">
         <v>391</v>
       </c>
@@ -3982,7 +4696,10 @@
         <v>563</v>
       </c>
     </row>
-    <row r="128" spans="2:5" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A128" s="3" t="s">
+        <v>689</v>
+      </c>
       <c r="B128" s="1" t="s">
         <v>393</v>
       </c>
@@ -3996,7 +4713,10 @@
         <v>564</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>690</v>
+      </c>
       <c r="B129" s="2" t="s">
         <v>395</v>
       </c>
@@ -4010,7 +4730,10 @@
         <v>566</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>691</v>
+      </c>
       <c r="B130" s="2" t="s">
         <v>397</v>
       </c>
@@ -4024,7 +4747,10 @@
         <v>567</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>692</v>
+      </c>
       <c r="B131" s="2" t="s">
         <v>399</v>
       </c>
@@ -4038,7 +4764,10 @@
         <v>568</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>693</v>
+      </c>
       <c r="B132" s="2" t="s">
         <v>421</v>
       </c>
@@ -4052,7 +4781,10 @@
         <v>487</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="3" t="s">
+        <v>694</v>
+      </c>
       <c r="B133" s="2" t="s">
         <v>424</v>
       </c>
@@ -4066,7 +4798,10 @@
         <v>487</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="3" t="s">
+        <v>695</v>
+      </c>
       <c r="B134" s="2" t="s">
         <v>425</v>
       </c>
@@ -4080,7 +4815,10 @@
         <v>538</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>696</v>
+      </c>
       <c r="B135" s="2" t="s">
         <v>427</v>
       </c>
@@ -4094,7 +4832,10 @@
         <v>569</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>697</v>
+      </c>
       <c r="B136" s="2" t="s">
         <v>430</v>
       </c>
@@ -4108,7 +4849,10 @@
         <v>545</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>698</v>
+      </c>
       <c r="B137" s="2" t="s">
         <v>432</v>
       </c>
@@ -4122,7 +4866,10 @@
         <v>570</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>699</v>
+      </c>
       <c r="B138" s="2" t="s">
         <v>434</v>
       </c>
@@ -4136,7 +4883,10 @@
         <v>496</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="3" t="s">
+        <v>700</v>
+      </c>
       <c r="B139" s="2" t="s">
         <v>436</v>
       </c>
@@ -4150,7 +4900,10 @@
         <v>571</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="3" t="s">
+        <v>701</v>
+      </c>
       <c r="B140" s="2" t="s">
         <v>437</v>
       </c>
@@ -4164,7 +4917,10 @@
         <v>572</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="3" t="s">
+        <v>702</v>
+      </c>
       <c r="B141" s="2" t="s">
         <v>440</v>
       </c>
@@ -4178,7 +4934,10 @@
         <v>573</v>
       </c>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="3" t="s">
+        <v>703</v>
+      </c>
       <c r="B142" s="2" t="s">
         <v>442</v>
       </c>
@@ -4192,7 +4951,10 @@
         <v>573</v>
       </c>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="3" t="s">
+        <v>704</v>
+      </c>
       <c r="B143" s="2" t="s">
         <v>455</v>
       </c>
@@ -4206,7 +4968,10 @@
         <v>574</v>
       </c>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="3" t="s">
+        <v>705</v>
+      </c>
       <c r="B144" s="2" t="s">
         <v>456</v>
       </c>
@@ -4220,7 +4985,10 @@
         <v>574</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="3" t="s">
+        <v>706</v>
+      </c>
       <c r="B145" s="2" t="s">
         <v>458</v>
       </c>
@@ -4234,7 +5002,10 @@
         <v>575</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="3" t="s">
+        <v>707</v>
+      </c>
       <c r="B146" s="2" t="s">
         <v>460</v>
       </c>
@@ -4248,7 +5019,10 @@
         <v>576</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="3" t="s">
+        <v>708</v>
+      </c>
       <c r="B147" s="2" t="s">
         <v>462</v>
       </c>
@@ -4262,7 +5036,10 @@
         <v>577</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>709</v>
+      </c>
       <c r="B148" s="2" t="s">
         <v>465</v>
       </c>
@@ -4276,7 +5053,10 @@
         <v>578</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>710</v>
+      </c>
       <c r="B149" s="2" t="s">
         <v>466</v>
       </c>
@@ -4290,7 +5070,10 @@
         <v>579</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>711</v>
+      </c>
       <c r="B150" s="2" t="s">
         <v>475</v>
       </c>
@@ -4304,7 +5087,10 @@
         <v>575</v>
       </c>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>712</v>
+      </c>
       <c r="B151" s="2" t="s">
         <v>477</v>
       </c>

</xml_diff>